<commit_message>
added some trade info
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBRandomTrade.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBRandomTrade.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,6 +448,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42633.676655092589</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>10022</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>304.83</v>
+      </c>
+      <c r="F4">
+        <v>303.5</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-0.44</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>